<commit_message>
Fixed bad Excel test fixture.
</commit_message>
<xml_diff>
--- a/tests/assets/secondary_task_with_google_sheets_and_excel_test/secondary_task_with_excel.xlsx
+++ b/tests/assets/secondary_task_with_google_sheets_and_excel_test/secondary_task_with_excel.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{B7C94A56-FAEA-4BD9-AE3C-5259F03F3C1D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DED06F3E-84C5-44E4-85D7-4C2A731E1127}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11895" windowHeight="16320" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="11895" windowHeight="16320" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="secondary" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="22">
   <si>
     <t>file</t>
   </si>
@@ -81,12 +81,18 @@
   </si>
   <si>
     <t>Excel - Secondary task test child 2 - parent 2</t>
+  </si>
+  <si>
+    <t>STTC-03</t>
+  </si>
+  <si>
+    <t>STTC-04</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -920,11 +926,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -981,7 +987,7 @@
         <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="D4" t="s">
         <v>14</v>
@@ -992,7 +998,7 @@
         <v>16</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
         <v>14</v>
@@ -1004,10 +1010,10 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>

</xml_diff>